<commit_message>
Final Updates (still need to clean data)
</commit_message>
<xml_diff>
--- a/Data/Detroit_Block_Groups_Table.xlsx
+++ b/Data/Detroit_Block_Groups_Table.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbmarks\Documents\GitHub\Geo572_Lab1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\GitHub\Geo572_Lab1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3828CBD5-645A-4942-B02D-AF0E4BD60D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10050"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detroit_Block_Groups_Table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -183,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -710,6 +719,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC4C4C4"/>
+      <color rgb="FF4C4C4C"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -766,7 +781,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -997,7 +1011,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1152,7 +1165,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1459,7 +1471,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1766,7 +1777,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2065,10 +2075,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="107"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="7"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2081,10 +2091,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="C4C4C4"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2093,12 +2100,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Mortgage Status by Selected Monthly Owner Costs as a Percentage of Household Income in the Past 12 Months</a:t>
+              <a:t>Selected Monthly Owner Costs as a Percentage of Household Income in the Past 12 Months</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2114,10 +2120,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C4C4C4"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2143,7 +2146,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent5">
+                <a:shade val="76000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2236,7 +2241,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent5">
+                <a:tint val="77000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2365,10 +2372,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="C4C4C4"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2406,6 +2410,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="C4C4C4"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Households</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="C4C4C4"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2424,10 +2477,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="C4C4C4"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2451,7 +2501,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2467,10 +2516,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C4C4C4"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2487,7 +2533,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:srgbClr val="4C4C4C"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2505,7 +2551,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:srgbClr val="C4C4C4"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2533,7 +2583,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2886,7 +2935,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3114,42 +3162,8 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -6230,7 +6244,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6260,7 +6280,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6290,7 +6316,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6320,7 +6352,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6338,19 +6376,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>185736</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>32610</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>45107</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6368,19 +6412,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6660,11 +6710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="Y22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>